<commit_message>
divide new vaccine into 1, 2 dose
</commit_message>
<xml_diff>
--- a/static/template_files/template-form-1.xlsx
+++ b/static/template_files/template-form-1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Ngày</t>
   </si>
@@ -55,7 +55,10 @@
     <t>F0 đang theo dõi tại khu cách ly</t>
   </si>
   <si>
-    <t>Vaccine tiêm trong ngày</t>
+    <t>Vaccine tiêm trong ngày (mũi 1 + mũi 2)</t>
+  </si>
+  <si>
+    <t>131274+10541</t>
   </si>
   <si>
     <t>Tổng số vaccine đã tiêm (mũi 1 + mũi 2)</t>
@@ -97,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,6 +108,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -400,19 +406,19 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
-        <v>140161.0</v>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>